<commit_message>
adapting to different xs
</commit_message>
<xml_diff>
--- a/tests/TestFiles/configuration/mainconfig.xlsx
+++ b/tests/TestFiles/configuration/mainconfig.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d.laghi\Documents\GitHub\JADE\Code\tests\TestFiles\configuration\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DATA\laghida\Documents\GitHub\JADE\tests\TestFiles\configuration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAE63A03-9487-4631-9F8E-8EE9B0ABD446}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B815A59-E3AE-4E43-B415-48CE81AC296F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{B0A3356C-3012-4321-B248-DE86B5D58E08}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{B0A3356C-3012-4321-B248-DE86B5D58E08}"/>
   </bookViews>
   <sheets>
     <sheet name="MAIN Config." sheetId="2" r:id="rId1"/>
@@ -37,10 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="64">
-  <si>
-    <t>xsdir Path</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="77">
   <si>
     <t>Default Benchmarks</t>
   </si>
@@ -51,12 +48,6 @@
     <t>Sphere.i</t>
   </si>
   <si>
-    <t>Run</t>
-  </si>
-  <si>
-    <t>True</t>
-  </si>
-  <si>
     <t>OnlyInput</t>
   </si>
   <si>
@@ -93,24 +84,9 @@
     <t>70c</t>
   </si>
   <si>
-    <t>multithread</t>
-  </si>
-  <si>
     <t>NPS cut-off</t>
   </si>
   <si>
-    <t>CTME cut-off</t>
-  </si>
-  <si>
-    <t>Relative Error cut-off</t>
-  </si>
-  <si>
-    <t>Code</t>
-  </si>
-  <si>
-    <t>Activation</t>
-  </si>
-  <si>
     <t>Default</t>
   </si>
   <si>
@@ -129,9 +105,6 @@
     <t>Computational benchmark additional options</t>
   </si>
   <si>
-    <t>CPU</t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
@@ -165,9 +138,6 @@
     <t>00c</t>
   </si>
   <si>
-    <t>C:\Users\d.laghi\Documents\MCNP\MCNP_DATA\xsdir_mcnp6.2</t>
-  </si>
-  <si>
     <t>HCPB_TBM_1D.i</t>
   </si>
   <si>
@@ -192,12 +162,6 @@
     <t>ITER_Cyl_SDDR.i</t>
   </si>
   <si>
-    <t>mcnp6</t>
-  </si>
-  <si>
-    <t>D1S5</t>
-  </si>
-  <si>
     <t>99c</t>
   </si>
   <si>
@@ -229,6 +193,81 @@
   </si>
   <si>
     <t>FENDL 3.2</t>
+  </si>
+  <si>
+    <t>MCNP executable</t>
+  </si>
+  <si>
+    <t>/home/mcnp/mcnpexecs/freia/mcnp6v2_ifort2020_openmpi4.1_220706</t>
+  </si>
+  <si>
+    <t>MCNP config</t>
+  </si>
+  <si>
+    <t>mcnp_config.sh</t>
+  </si>
+  <si>
+    <t>Serpent executable</t>
+  </si>
+  <si>
+    <t>/home/sbradnam/Software/freia/Serpent2_src/v2.1.32_ccfe/sss2</t>
+  </si>
+  <si>
+    <t>Serpent config</t>
+  </si>
+  <si>
+    <t>serpent_config.sh</t>
+  </si>
+  <si>
+    <t>OpenMC executable</t>
+  </si>
+  <si>
+    <t>/home/sbradnam/Software/freia/OPENMC_311022/openmc/build/bin/openmc</t>
+  </si>
+  <si>
+    <t>OpenMC config</t>
+  </si>
+  <si>
+    <t>openmc_config.sh</t>
+  </si>
+  <si>
+    <t>d1S executable</t>
+  </si>
+  <si>
+    <t>d1S config</t>
+  </si>
+  <si>
+    <t>OpenMP threads</t>
+  </si>
+  <si>
+    <t>MPI tasks</t>
+  </si>
+  <si>
+    <t>Batch system</t>
+  </si>
+  <si>
+    <t>llsubmit</t>
+  </si>
+  <si>
+    <t>Batch file</t>
+  </si>
+  <si>
+    <t>Job_Script_Templates/LLtemplate.cmd</t>
+  </si>
+  <si>
+    <t>Folder Name</t>
+  </si>
+  <si>
+    <t>MCNP</t>
+  </si>
+  <si>
+    <t>Serpent</t>
+  </si>
+  <si>
+    <t>OpenMC</t>
+  </si>
+  <si>
+    <t>d1S</t>
   </si>
 </sst>
 </file>
@@ -303,7 +342,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -382,11 +421,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -461,9 +513,15 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -479,7 +537,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -775,70 +833,122 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6A1A2DE-3EB8-4AD4-9CF1-023800AFF144}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="37.44140625" customWidth="1"/>
+    <col min="1" max="1" width="37.453125" customWidth="1"/>
     <col min="2" max="2" width="106" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="31.8" thickBot="1" x14ac:dyDescent="0.65">
+    <row r="1" spans="1:2" ht="31.5" thickBot="1" x14ac:dyDescent="0.75">
       <c r="A1" s="22" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="B1" s="23"/>
     </row>
-    <row r="2" spans="1:2" ht="18" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="18" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" ht="18.5" hidden="1" x14ac:dyDescent="0.45">
+      <c r="A2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A3" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A4" s="3" t="s">
-        <v>18</v>
+        <v>54</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="18.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A5" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B5" s="6">
+        <v>56</v>
+      </c>
+      <c r="B5" s="28" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="18.5" hidden="1" x14ac:dyDescent="0.45">
+      <c r="A6" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A7" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A8" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A9" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="B9" s="28"/>
+    </row>
+    <row r="10" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A10" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="B10" s="28"/>
+    </row>
+    <row r="11" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A11" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="B11" s="28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A12" s="29" t="s">
+        <v>67</v>
+      </c>
+      <c r="B12" s="28">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="18" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="18.600000000000001" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>28</v>
+    <row r="13" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A13" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="B13" s="28" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="19" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A14" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -854,28 +964,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51291A71-4ED6-4F39-B575-920D7DB78E56}">
   <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView topLeftCell="G2" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="24.77734375" style="20" customWidth="1"/>
-    <col min="2" max="2" width="14.88671875" style="14" customWidth="1"/>
-    <col min="3" max="3" width="11.21875" style="14" customWidth="1"/>
-    <col min="4" max="4" width="9.44140625" style="14" customWidth="1"/>
-    <col min="5" max="5" width="10" style="14" customWidth="1"/>
-    <col min="6" max="6" width="8.88671875" style="14" customWidth="1"/>
-    <col min="7" max="7" width="8.44140625" style="14" customWidth="1"/>
-    <col min="8" max="8" width="11.109375" style="14" customWidth="1"/>
-    <col min="9" max="9" width="9" style="14" customWidth="1"/>
-    <col min="10" max="10" width="8.88671875" style="18"/>
-    <col min="11" max="16384" width="8.88671875" style="14"/>
+    <col min="1" max="1" width="24.81640625" style="20" customWidth="1"/>
+    <col min="2" max="2" width="14.90625" style="14" customWidth="1"/>
+    <col min="3" max="3" width="11.1796875" style="14" customWidth="1"/>
+    <col min="4" max="7" width="9.453125" style="14" customWidth="1"/>
+    <col min="8" max="8" width="10" style="14" customWidth="1"/>
+    <col min="9" max="9" width="8.90625" style="14" customWidth="1"/>
+    <col min="10" max="10" width="9" style="14" customWidth="1"/>
+    <col min="11" max="16384" width="8.90625" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="31" x14ac:dyDescent="0.35">
       <c r="A1" s="25" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="B1" s="25"/>
       <c r="C1" s="25"/>
@@ -887,9 +994,9 @@
       <c r="I1" s="25"/>
       <c r="J1" s="25"/>
     </row>
-    <row r="2" spans="1:10" s="15" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" s="15" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="24" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" s="24"/>
       <c r="C2" s="24"/>
@@ -901,225 +1008,253 @@
       <c r="I2" s="24"/>
       <c r="J2" s="24"/>
     </row>
-    <row r="3" spans="1:10" s="20" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" s="20" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="16" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="B3" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="E3" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="F3" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="G3" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="H3" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="I3" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="J3" s="16" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A4" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="G3" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="H3" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="I3" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="J3" s="16" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="B4" s="18" t="s">
-        <v>3</v>
-      </c>
       <c r="C4" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="H4" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="I4" s="19">
+        <v>10000</v>
+      </c>
+      <c r="J4" s="18">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A5" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="H5" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="I5" s="19">
+        <v>10000</v>
+      </c>
+      <c r="J5" s="18"/>
+    </row>
+    <row r="6" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A6" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="G6" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="H6" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="I6" s="19">
+        <v>1000</v>
+      </c>
+      <c r="J6" s="18"/>
+    </row>
+    <row r="7" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A7" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="D4" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="E4" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="F4" s="19">
-        <v>10000</v>
-      </c>
-      <c r="G4" s="18"/>
-      <c r="H4" s="18"/>
-      <c r="I4" s="18">
+      <c r="B7" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="G7" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="H7" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="I7" s="19">
+        <v>1000</v>
+      </c>
+      <c r="J7" s="18"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A8" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="F8" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="G8" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="H8" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="I8" s="19">
+        <v>1000</v>
+      </c>
+      <c r="J8" s="18"/>
+    </row>
+    <row r="9" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A9" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="F9" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="G9" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="H9" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="I9" s="19">
+        <v>1000000</v>
+      </c>
+      <c r="J9" s="18"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A10" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="F10" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="G10" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="H10" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="I10" s="19">
+        <v>100000000</v>
+      </c>
+      <c r="J10" s="18">
         <v>5</v>
       </c>
-      <c r="J4" s="18" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="B5" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="C5" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="D5" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="E5" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="F5" s="19">
-        <v>10000</v>
-      </c>
-      <c r="G5" s="18"/>
-      <c r="H5" s="18"/>
-      <c r="I5" s="18"/>
-      <c r="J5" s="18" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="B6" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="C6" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="D6" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="E6" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="F6" s="19">
-        <v>1000</v>
-      </c>
-      <c r="G6" s="18"/>
-      <c r="H6" s="18"/>
-      <c r="I6" s="18"/>
-      <c r="J6" s="18" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="17" t="s">
-        <v>45</v>
-      </c>
-      <c r="B7" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="C7" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="D7" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="E7" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="F7" s="19">
-        <v>1000</v>
-      </c>
-      <c r="G7" s="18"/>
-      <c r="H7" s="18"/>
-      <c r="I7" s="18"/>
-      <c r="J7" s="18" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" s="17" t="s">
-        <v>48</v>
-      </c>
-      <c r="B8" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="C8" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="D8" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="E8" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="F8" s="19">
-        <v>1000</v>
-      </c>
-      <c r="G8" s="18"/>
-      <c r="H8" s="18"/>
-      <c r="I8" s="18"/>
-      <c r="J8" s="18" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" s="17" t="s">
-        <v>49</v>
-      </c>
-      <c r="B9" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="C9" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="D9" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="E9" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="F9" s="19">
-        <v>1000000</v>
-      </c>
-      <c r="G9" s="18"/>
-      <c r="H9" s="18"/>
-      <c r="I9" s="18"/>
-      <c r="J9" s="18" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="B10" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="C10" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="D10" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="E10" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="F10" s="19">
-        <v>100000000</v>
-      </c>
-      <c r="G10" s="18"/>
-      <c r="H10" s="18"/>
-      <c r="I10" s="18">
-        <v>5</v>
-      </c>
-      <c r="J10" s="18" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" s="17"/>
       <c r="B11" s="18"/>
       <c r="C11" s="18"/>
@@ -1129,6 +1264,7 @@
       <c r="G11" s="18"/>
       <c r="H11" s="18"/>
       <c r="I11" s="18"/>
+      <c r="J11" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1145,26 +1281,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8EEB530-2BB1-44BD-96B5-AB98331CD0CC}">
   <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="38" customWidth="1"/>
-    <col min="2" max="2" width="13.5546875" customWidth="1"/>
-    <col min="3" max="3" width="13.109375" customWidth="1"/>
-    <col min="4" max="4" width="9.44140625" customWidth="1"/>
-    <col min="5" max="5" width="16.33203125" customWidth="1"/>
-    <col min="6" max="6" width="13.6640625" customWidth="1"/>
-    <col min="7" max="7" width="18.109375" customWidth="1"/>
-    <col min="8" max="9" width="21.109375" customWidth="1"/>
-    <col min="10" max="10" width="8.88671875" style="11"/>
+    <col min="2" max="2" width="13.54296875" customWidth="1"/>
+    <col min="3" max="3" width="13.08984375" customWidth="1"/>
+    <col min="4" max="7" width="9.453125" customWidth="1"/>
+    <col min="8" max="8" width="16.36328125" customWidth="1"/>
+    <col min="9" max="9" width="13.6328125" customWidth="1"/>
+    <col min="10" max="10" width="21.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="31.2" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:10" ht="31" x14ac:dyDescent="0.7">
       <c r="A1" s="27" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="B1" s="27"/>
       <c r="C1" s="27"/>
@@ -1176,9 +1310,9 @@
       <c r="I1" s="27"/>
       <c r="J1" s="27"/>
     </row>
-    <row r="2" spans="1:10" s="8" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" s="8" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="26" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" s="26"/>
       <c r="C2" s="26"/>
@@ -1190,91 +1324,99 @@
       <c r="I2" s="26"/>
       <c r="J2" s="26"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="G3" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="H3" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="I3" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="J3" s="13" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A4" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="G3" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="H3" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="I3" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="J3" s="13" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>40</v>
-      </c>
       <c r="C4" s="21" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="E4" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="F4" s="12">
+        <v>25</v>
+      </c>
+      <c r="E4" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="F4" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="G4" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="I4" s="12">
         <v>1000000</v>
       </c>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="11" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J4" s="11"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="11" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="C5" s="21" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="E5" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="F5" s="12">
+        <v>26</v>
+      </c>
+      <c r="E5" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="F5" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="G5" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="I5" s="12">
         <v>10000</v>
       </c>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="11"/>
-      <c r="J5" s="11" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J5" s="11"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" s="11"/>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
@@ -1284,8 +1426,9 @@
       <c r="G6" s="11"/>
       <c r="H6" s="11"/>
       <c r="I6" s="11"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J6" s="11"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" s="11"/>
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
@@ -1295,8 +1438,9 @@
       <c r="G7" s="11"/>
       <c r="H7" s="11"/>
       <c r="I7" s="11"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J7" s="11"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" s="11"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
@@ -1306,8 +1450,9 @@
       <c r="G8" s="11"/>
       <c r="H8" s="11"/>
       <c r="I8" s="11"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J8" s="11"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" s="11"/>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
@@ -1317,6 +1462,7 @@
       <c r="G9" s="11"/>
       <c r="H9" s="11"/>
       <c r="I9" s="11"/>
+      <c r="J9" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1330,94 +1476,110 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27F03233-EAF0-4262-AA38-EF4B945A3E70}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="1"/>
-    <col min="2" max="2" width="18.109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8.90625" style="1"/>
+    <col min="2" max="2" width="18.08984375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="39.36328125" customWidth="1"/>
+    <col min="5" max="5" width="31.90625" customWidth="1"/>
+    <col min="6" max="6" width="25.08984375" customWidth="1"/>
+    <col min="7" max="7" width="36" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="10" t="s">
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="B4" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
+      <c r="C7" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C7" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>53</v>
-      </c>
       <c r="B8" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed testrun except D1S
</commit_message>
<xml_diff>
--- a/tests/TestFiles/configuration/mainconfig.xlsx
+++ b/tests/TestFiles/configuration/mainconfig.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DATA\laghida\Documents\GitHub\JADE\tests\TestFiles\configuration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20FA00FC-6A5A-4851-854C-89ECAD261EF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F47B15A1-8856-466E-A52D-A86D64D33909}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1520" yWindow="1520" windowWidth="14400" windowHeight="7360" firstSheet="1" activeTab="2" xr2:uid="{B0A3356C-3012-4321-B248-DE86B5D58E08}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="1" xr2:uid="{B0A3356C-3012-4321-B248-DE86B5D58E08}"/>
   </bookViews>
   <sheets>
     <sheet name="MAIN Config." sheetId="2" r:id="rId1"/>
@@ -42,9 +42,6 @@
     <t>Default Benchmarks</t>
   </si>
   <si>
-    <t>Sphere.i</t>
-  </si>
-  <si>
     <t>OnlyInput</t>
   </si>
   <si>
@@ -117,9 +114,6 @@
     <t>false</t>
   </si>
   <si>
-    <t>ITER_1D.i</t>
-  </si>
-  <si>
     <t>ITER 1D (by M. Sawan)</t>
   </si>
   <si>
@@ -135,30 +129,18 @@
     <t>00c</t>
   </si>
   <si>
-    <t>HCPB_TBM_1D.i</t>
-  </si>
-  <si>
     <t>Helium Cooled Pebble Bed Test Blanket Module (1D)</t>
   </si>
   <si>
     <t>Water Cooled Lithium Lead Test Blanket Module (1D)</t>
   </si>
   <si>
-    <t>WCLL_TBM_1D.i</t>
-  </si>
-  <si>
-    <t>C_Model.i</t>
-  </si>
-  <si>
     <t>C-Model R181031 rev190715</t>
   </si>
   <si>
     <t>ITER Cylindrical benchmark for SDDR</t>
   </si>
   <si>
-    <t>ITER_Cyl_SDDR.i</t>
-  </si>
-  <si>
     <t>99c</t>
   </si>
   <si>
@@ -168,9 +150,6 @@
     <t>Sphere SDDR</t>
   </si>
   <si>
-    <t>SphereSDDR.i</t>
-  </si>
-  <si>
     <t>Custom Input</t>
   </si>
   <si>
@@ -265,6 +244,27 @@
   </si>
   <si>
     <t>d1S</t>
+  </si>
+  <si>
+    <t>Sphere</t>
+  </si>
+  <si>
+    <t>ITER_1D</t>
+  </si>
+  <si>
+    <t>HCPB_TBM_1D</t>
+  </si>
+  <si>
+    <t>WCLL_TBM_1D</t>
+  </si>
+  <si>
+    <t>C_Model</t>
+  </si>
+  <si>
+    <t>ITER_Cyl_SDDR</t>
+  </si>
+  <si>
+    <t>SphereSDDR</t>
   </si>
 </sst>
 </file>
@@ -435,7 +435,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -456,7 +456,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -471,9 +470,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -489,9 +485,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -504,16 +497,16 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -843,109 +836,109 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="31.5" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="A1" s="24" t="s">
-        <v>17</v>
-      </c>
-      <c r="B1" s="25"/>
+      <c r="A1" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="22"/>
     </row>
     <row r="2" spans="1:2" ht="18.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>18</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A4" s="3" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="18.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A5" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="B5" s="22" t="s">
-        <v>56</v>
+        <v>48</v>
+      </c>
+      <c r="B5" s="19" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="18.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A6" s="3" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A7" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A8" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A9" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="B9" s="19"/>
+    </row>
+    <row r="10" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A10" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B10" s="19"/>
+    </row>
+    <row r="11" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A11" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="B11" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A12" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B12" s="19">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A13" s="20" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A8" s="23" t="s">
+      <c r="B13" s="19" t="s">
         <v>61</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A9" s="23" t="s">
-        <v>63</v>
-      </c>
-      <c r="B9" s="22"/>
-    </row>
-    <row r="10" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A10" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="B10" s="22"/>
-    </row>
-    <row r="11" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A11" s="23" t="s">
-        <v>65</v>
-      </c>
-      <c r="B11" s="22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A12" s="23" t="s">
-        <v>66</v>
-      </c>
-      <c r="B12" s="22">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A13" s="23" t="s">
-        <v>67</v>
-      </c>
-      <c r="B13" s="22" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="19" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A14" s="4" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -961,307 +954,307 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51291A71-4ED6-4F39-B575-920D7DB78E56}">
   <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="24.81640625" style="20" customWidth="1"/>
-    <col min="2" max="2" width="14.90625" style="14" customWidth="1"/>
-    <col min="3" max="3" width="11.1796875" style="14" customWidth="1"/>
-    <col min="4" max="7" width="9.453125" style="14" customWidth="1"/>
-    <col min="8" max="8" width="10" style="14" customWidth="1"/>
-    <col min="9" max="9" width="8.90625" style="14" customWidth="1"/>
-    <col min="10" max="10" width="9" style="14" customWidth="1"/>
-    <col min="11" max="16384" width="8.90625" style="14"/>
+    <col min="1" max="1" width="24.81640625" style="18" customWidth="1"/>
+    <col min="2" max="2" width="14.90625" style="13" customWidth="1"/>
+    <col min="3" max="3" width="11.1796875" style="13" customWidth="1"/>
+    <col min="4" max="7" width="9.453125" style="13" customWidth="1"/>
+    <col min="8" max="8" width="10" style="13" customWidth="1"/>
+    <col min="9" max="9" width="8.90625" style="13" customWidth="1"/>
+    <col min="10" max="10" width="9" style="13" customWidth="1"/>
+    <col min="11" max="16384" width="8.90625" style="13"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31" x14ac:dyDescent="0.35">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+    </row>
+    <row r="2" spans="1:10" ht="27" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="23"/>
+    </row>
+    <row r="3" spans="1:10" s="18" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A3" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-    </row>
-    <row r="2" spans="1:10" s="15" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="26" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="26"/>
-      <c r="J2" s="26"/>
-    </row>
-    <row r="3" spans="1:10" s="20" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A3" s="16" t="s">
+      <c r="B3" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="H3" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="I3" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="J3" s="14" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A4" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B4" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="I4" s="17">
+        <v>10000</v>
+      </c>
+      <c r="J4" s="16">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A5" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="H5" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="I5" s="17">
+        <v>10000</v>
+      </c>
+      <c r="J5" s="16"/>
+    </row>
+    <row r="6" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A6" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="C3" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="16" t="s">
+      <c r="C6" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="G6" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="H6" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="I6" s="17">
+        <v>1000</v>
+      </c>
+      <c r="J6" s="16"/>
+    </row>
+    <row r="7" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A7" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="E3" s="16" t="s">
+      <c r="C7" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="G7" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="H7" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="I7" s="17">
+        <v>1000</v>
+      </c>
+      <c r="J7" s="16"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A8" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="F3" s="16" t="s">
+      <c r="C8" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="G8" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="H8" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="I8" s="17">
+        <v>1000</v>
+      </c>
+      <c r="J8" s="16"/>
+    </row>
+    <row r="9" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A9" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="G3" s="16" t="s">
+      <c r="C9" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="G9" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="H9" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="I9" s="17">
+        <v>1000000</v>
+      </c>
+      <c r="J9" s="16"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A10" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="H3" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="I3" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="J3" s="16" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A4" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="E4" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="F4" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="G4" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="H4" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="I4" s="19">
-        <v>10000</v>
-      </c>
-      <c r="J4" s="18">
+      <c r="C10" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="F10" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="G10" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="H10" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="I10" s="17">
+        <v>100000000</v>
+      </c>
+      <c r="J10" s="16">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A5" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="B5" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="D5" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="E5" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="F5" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="G5" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="H5" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="I5" s="19">
-        <v>10000</v>
-      </c>
-      <c r="J5" s="18"/>
-    </row>
-    <row r="6" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A6" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="B6" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="C6" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="D6" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="E6" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="F6" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="G6" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="H6" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="I6" s="19">
-        <v>1000</v>
-      </c>
-      <c r="J6" s="18"/>
-    </row>
-    <row r="7" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A7" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="B7" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="C7" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="D7" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="E7" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="F7" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="G7" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="H7" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="I7" s="19">
-        <v>1000</v>
-      </c>
-      <c r="J7" s="18"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A8" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="B8" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="C8" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="E8" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="F8" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="G8" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="H8" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="I8" s="19">
-        <v>1000</v>
-      </c>
-      <c r="J8" s="18"/>
-    </row>
-    <row r="9" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A9" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="B9" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="C9" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="E9" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="F9" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="G9" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="H9" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="I9" s="19">
-        <v>1000000</v>
-      </c>
-      <c r="J9" s="18"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A10" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="B10" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="C10" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="D10" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="E10" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="F10" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="G10" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="H10" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="I10" s="19">
-        <v>100000000</v>
-      </c>
-      <c r="J10" s="18">
-        <v>5</v>
-      </c>
-    </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A11" s="17"/>
-      <c r="B11" s="18"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="18"/>
-      <c r="H11" s="18"/>
-      <c r="I11" s="18"/>
-      <c r="J11" s="18"/>
+      <c r="A11" s="15"/>
+      <c r="B11" s="16"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="16"/>
+      <c r="J11" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1278,7 +1271,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8EEB530-2BB1-44BD-96B5-AB98331CD0CC}">
   <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -1294,172 +1287,172 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31" x14ac:dyDescent="0.7">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+    </row>
+    <row r="2" spans="1:10" ht="27" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A2" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A3" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
-      <c r="J1" s="29"/>
-    </row>
-    <row r="2" spans="1:10" s="8" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="28" t="s">
+      <c r="B3" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="I3" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="J3" s="12" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A4" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28"/>
-      <c r="I2" s="28"/>
-      <c r="J2" s="28"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A3" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="C3" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="E3" s="13" t="s">
-        <v>73</v>
-      </c>
-      <c r="F3" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="G3" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="H3" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="I3" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="J3" s="13" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A4" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="C4" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="E4" s="11" t="b">
+      <c r="F4" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="F4" s="11" t="b">
+      <c r="G4" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="G4" s="11" t="b">
+      <c r="H4" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="I4" s="11">
+        <v>1000000</v>
+      </c>
+      <c r="J4" s="10"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A5" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="H4" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="I4" s="12">
-        <v>1000000</v>
-      </c>
-      <c r="J4" s="11"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A5" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="C5" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="E5" s="11" t="b">
+      <c r="F5" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="F5" s="11" t="b">
+      <c r="G5" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="G5" s="11" t="b">
-        <v>0</v>
-      </c>
-      <c r="H5" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="I5" s="12">
+      <c r="H5" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="I5" s="11">
         <v>10000</v>
       </c>
-      <c r="J5" s="11"/>
+      <c r="J5" s="10"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A6" s="11"/>
-      <c r="B6" s="11"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="11"/>
-      <c r="J6" s="11"/>
+      <c r="A6" s="10"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="10"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A7" s="11"/>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="11"/>
-      <c r="J7" s="11"/>
+      <c r="A7" s="10"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="10"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A8" s="11"/>
-      <c r="B8" s="11"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="11"/>
-      <c r="I8" s="11"/>
-      <c r="J8" s="11"/>
+      <c r="A8" s="10"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A9" s="11"/>
-      <c r="B9" s="11"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11"/>
-      <c r="I9" s="11"/>
-      <c r="J9" s="11"/>
+      <c r="A9" s="10"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1490,93 +1483,93 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="G1" s="9" t="s">
-        <v>75</v>
+      <c r="C1" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed tests missing new keyword in config files
</commit_message>
<xml_diff>
--- a/tests/TestFiles/configuration/mainconfig.xlsx
+++ b/tests/TestFiles/configuration/mainconfig.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DATA\laghida\Documents\GitHub\JADE\tests\TestFiles\configuration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F47B15A1-8856-466E-A52D-A86D64D33909}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{088F89AD-9A0B-4A71-B75F-D3827C36FA95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="1" xr2:uid="{B0A3356C-3012-4321-B248-DE86B5D58E08}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B0A3356C-3012-4321-B248-DE86B5D58E08}"/>
   </bookViews>
   <sheets>
     <sheet name="MAIN Config." sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="77">
   <si>
     <t>Default Benchmarks</t>
   </si>
@@ -265,6 +265,9 @@
   </si>
   <si>
     <t>SphereSDDR</t>
+  </si>
+  <si>
+    <t>MPI executable prefix</t>
   </si>
 </sst>
 </file>
@@ -823,10 +826,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6A1A2DE-3EB8-4AD4-9CF1-023800AFF144}">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -927,17 +930,23 @@
     </row>
     <row r="13" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A13" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="B13" s="19"/>
+    </row>
+    <row r="14" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A14" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="B13" s="19" t="s">
+      <c r="B14" s="19" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="19" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A14" s="4" t="s">
+    <row r="15" spans="1:2" ht="19" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A15" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B15" s="7" t="s">
         <v>63</v>
       </c>
     </row>
@@ -954,7 +963,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51291A71-4ED6-4F39-B575-920D7DB78E56}">
   <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>

</xml_diff>